<commit_message>
fixed creating excel when running with exe
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -415,7 +415,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:W12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -423,9 +423,16 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="12.65" customWidth="1" min="3" max="3"/>
+    <col width="21.85" customWidth="1" min="3" max="3"/>
     <col width="6.899999999999999" customWidth="1" min="4" max="4"/>
-    <col width="9.199999999999999" customWidth="1" min="5" max="5"/>
+    <col width="10.35" customWidth="1" min="5" max="5"/>
+    <col width="8.049999999999999" customWidth="1" min="7" max="7"/>
+    <col width="10.35" customWidth="1" min="11" max="11"/>
+    <col width="6.899999999999999" customWidth="1" min="12" max="12"/>
+    <col width="10.35" customWidth="1" min="13" max="13"/>
+    <col width="17.25" customWidth="1" min="15" max="15"/>
+    <col width="14.95" customWidth="1" min="19" max="19"/>
+    <col width="18.4" customWidth="1" min="23" max="23"/>
   </cols>
   <sheetData>
     <row r="1"/>
@@ -438,6 +445,31 @@
           <t>Monday</t>
         </is>
       </c>
+      <c r="G5" s="1" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="K5" s="1" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="O5" s="1" t="inlineStr">
+        <is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="S5" s="1" t="inlineStr">
+        <is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="W5" s="1" t="inlineStr">
+        <is>
+          <t>Saturday</t>
+        </is>
+      </c>
     </row>
     <row r="6"/>
     <row r="7">
@@ -446,6 +478,31 @@
           <t>Chest</t>
         </is>
       </c>
+      <c r="G7" s="1" t="inlineStr">
+        <is>
+          <t>Back</t>
+        </is>
+      </c>
+      <c r="K7" s="1" t="inlineStr">
+        <is>
+          <t>Shoulder</t>
+        </is>
+      </c>
+      <c r="O7" s="1" t="inlineStr">
+        <is>
+          <t>Chest &amp; Triceps</t>
+        </is>
+      </c>
+      <c r="S7" s="1" t="inlineStr">
+        <is>
+          <t>Back &amp; Biceps</t>
+        </is>
+      </c>
+      <c r="W7" s="1" t="inlineStr">
+        <is>
+          <t>Legs &amp; Shoulders</t>
+        </is>
+      </c>
     </row>
     <row r="8"/>
     <row r="9">
@@ -456,12 +513,67 @@
       </c>
       <c r="D9" s="1" t="inlineStr">
         <is>
+          <t>4 sets</t>
+        </is>
+      </c>
+      <c r="E9" s="1" t="inlineStr">
+        <is>
+          <t>8-12 reps</t>
+        </is>
+      </c>
+      <c r="K9" s="1" t="inlineStr">
+        <is>
+          <t>Box style</t>
+        </is>
+      </c>
+      <c r="L9" s="1" t="inlineStr">
+        <is>
+          <t>4 sets</t>
+        </is>
+      </c>
+      <c r="M9" s="1" t="inlineStr">
+        <is>
+          <t>8-12 reps</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="C10" s="1" t="inlineStr">
+        <is>
+          <t>Incline Bench Press</t>
+        </is>
+      </c>
+      <c r="D10" s="1" t="inlineStr">
+        <is>
           <t>3 sets</t>
         </is>
       </c>
-      <c r="E9" s="1" t="inlineStr">
-        <is>
-          <t>4-8 reps</t>
+      <c r="E10" s="1" t="inlineStr">
+        <is>
+          <t>4-6 reps</t>
+        </is>
+      </c>
+      <c r="K10" s="1" t="inlineStr">
+        <is>
+          <t>Jog</t>
+        </is>
+      </c>
+      <c r="L10" s="1" t="inlineStr">
+        <is>
+          <t>3 sets</t>
+        </is>
+      </c>
+      <c r="M10" s="1" t="inlineStr">
+        <is>
+          <t>4-6 reps</t>
+        </is>
+      </c>
+    </row>
+    <row r="11"/>
+    <row r="12">
+      <c r="W12" s="1" t="inlineStr">
+        <is>
+          <t>Abs</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
code refacotirng and fixes
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -45,7 +45,8 @@
       <b val="1"/>
     </font>
     <font>
-      <color rgb="00FFFFFF"/>
+      <b val="1"/>
+      <color rgb="00000000"/>
       <sz val="13"/>
     </font>
   </fonts>
@@ -191,84 +192,44 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table0" displayName="Table0" ref="C9:E11" headerRowCount="1">
-  <autoFilter ref="C9:E11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table0" displayName="Table0" ref="C9:E12" headerRowCount="0">
   <tableColumns count="3">
-    <tableColumn id="3" name="Exercises"/>
-    <tableColumn id="4" name="Sets"/>
-    <tableColumn id="5" name="Reps"/>
+    <tableColumn id="3" name="Column3"/>
+    <tableColumn id="4" name="Column4"/>
+    <tableColumn id="5" name="Column5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table1" displayName="Table1" ref="G9:I11" headerRowCount="1">
-  <autoFilter ref="G9:I11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table1" displayName="Table1" ref="C19:E22" headerRowCount="0">
   <tableColumns count="3">
-    <tableColumn id="7" name="Exercises"/>
-    <tableColumn id="8" name="Sets"/>
-    <tableColumn id="9" name="Reps"/>
+    <tableColumn id="3" name="Column3"/>
+    <tableColumn id="4" name="Column4"/>
+    <tableColumn id="5" name="Column5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table2" displayName="Table2" ref="K9:M11" headerRowCount="1">
-  <autoFilter ref="K9:M11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table2" displayName="Table2" ref="G9:I11" headerRowCount="0">
   <tableColumns count="3">
-    <tableColumn id="11" name="Exercises"/>
-    <tableColumn id="12" name="Sets"/>
-    <tableColumn id="13" name="Reps"/>
+    <tableColumn id="7" name="Column7"/>
+    <tableColumn id="8" name="Column8"/>
+    <tableColumn id="9" name="Column9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table3" displayName="Table3" ref="O9:Q11" headerRowCount="1">
-  <autoFilter ref="O9:Q11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table3" displayName="Table3" ref="K9:M11" headerRowCount="0">
   <tableColumns count="3">
-    <tableColumn id="15" name="Exercises"/>
-    <tableColumn id="16" name="Sets"/>
-    <tableColumn id="17" name="Reps"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table4" displayName="Table4" ref="S9:U11" headerRowCount="1">
-  <autoFilter ref="S9:U11"/>
-  <tableColumns count="3">
-    <tableColumn id="19" name="Exercises"/>
-    <tableColumn id="20" name="Sets"/>
-    <tableColumn id="21" name="Reps"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table5" displayName="Table5" ref="W9:Y11" headerRowCount="1">
-  <autoFilter ref="W9:Y11"/>
-  <tableColumns count="3">
-    <tableColumn id="23" name="Exercises"/>
-    <tableColumn id="24" name="Sets"/>
-    <tableColumn id="25" name="Reps"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table6" displayName="Table6" ref="W19:Y21" headerRowCount="1">
-  <autoFilter ref="W19:Y21"/>
-  <tableColumns count="3">
-    <tableColumn id="23" name="Exercises"/>
-    <tableColumn id="24" name="Sets"/>
-    <tableColumn id="25" name="Reps"/>
+    <tableColumn id="11" name="Column11"/>
+    <tableColumn id="12" name="Column12"/>
+    <tableColumn id="13" name="Column13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
 </table>
@@ -563,7 +524,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y20"/>
+  <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -571,24 +532,15 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="13.75" customWidth="1" min="3" max="3"/>
-    <col width="6.25" customWidth="1" min="4" max="4"/>
-    <col width="5" customWidth="1" min="5" max="5"/>
-    <col width="23.75" customWidth="1" min="7" max="7"/>
-    <col width="5" customWidth="1" min="8" max="8"/>
-    <col width="5" customWidth="1" min="9" max="9"/>
-    <col width="11.25" customWidth="1" min="11" max="11"/>
-    <col width="10" customWidth="1" min="12" max="12"/>
-    <col width="5" customWidth="1" min="13" max="13"/>
-    <col width="11.25" customWidth="1" min="15" max="15"/>
-    <col width="18.75" customWidth="1" min="16" max="16"/>
-    <col width="5" customWidth="1" min="17" max="17"/>
-    <col width="11.25" customWidth="1" min="19" max="19"/>
-    <col width="16.25" customWidth="1" min="20" max="20"/>
-    <col width="5" customWidth="1" min="21" max="21"/>
-    <col width="11.25" customWidth="1" min="23" max="23"/>
-    <col width="20" customWidth="1" min="24" max="24"/>
-    <col width="5" customWidth="1" min="25" max="25"/>
+    <col width="30.4" customWidth="1" min="3" max="3"/>
+    <col width="11.2" customWidth="1" min="4" max="4"/>
+    <col width="6.4" customWidth="1" min="5" max="5"/>
+    <col width="14.4" customWidth="1" min="7" max="7"/>
+    <col width="6.4" customWidth="1" min="8" max="8"/>
+    <col width="6.4" customWidth="1" min="9" max="9"/>
+    <col width="14.4" customWidth="1" min="11" max="11"/>
+    <col width="9.600000000000001" customWidth="1" min="12" max="12"/>
+    <col width="6.4" customWidth="1" min="13" max="13"/>
   </cols>
   <sheetData>
     <row r="1"/>
@@ -605,39 +557,18 @@
       <c r="E5" s="2" t="n"/>
       <c r="G5" s="1" t="inlineStr">
         <is>
-          <t>Tuesday</t>
+          <t>Wednesday</t>
         </is>
       </c>
       <c r="H5" s="2" t="n"/>
       <c r="I5" s="2" t="n"/>
       <c r="K5" s="1" t="inlineStr">
         <is>
-          <t>Wednesday</t>
+          <t>Friday</t>
         </is>
       </c>
       <c r="L5" s="2" t="n"/>
       <c r="M5" s="2" t="n"/>
-      <c r="O5" s="1" t="inlineStr">
-        <is>
-          <t>Thursday</t>
-        </is>
-      </c>
-      <c r="P5" s="2" t="n"/>
-      <c r="Q5" s="2" t="n"/>
-      <c r="S5" s="1" t="inlineStr">
-        <is>
-          <t>Friday</t>
-        </is>
-      </c>
-      <c r="T5" s="2" t="n"/>
-      <c r="U5" s="2" t="n"/>
-      <c r="W5" s="1" t="inlineStr">
-        <is>
-          <t>Saturday</t>
-        </is>
-      </c>
-      <c r="X5" s="2" t="n"/>
-      <c r="Y5" s="2" t="n"/>
     </row>
     <row r="6"/>
     <row r="7">
@@ -658,7 +589,7 @@
       </c>
       <c r="H7" s="4" t="inlineStr">
         <is>
-          <t>Back</t>
+          <t>Legs</t>
         </is>
       </c>
       <c r="K7" s="3" t="inlineStr">
@@ -668,37 +599,7 @@
       </c>
       <c r="L7" s="4" t="inlineStr">
         <is>
-          <t>Shoulder</t>
-        </is>
-      </c>
-      <c r="O7" s="3" t="inlineStr">
-        <is>
-          <t>Workout:</t>
-        </is>
-      </c>
-      <c r="P7" s="4" t="inlineStr">
-        <is>
-          <t>Chest &amp; Triceps</t>
-        </is>
-      </c>
-      <c r="S7" s="3" t="inlineStr">
-        <is>
-          <t>Workout:</t>
-        </is>
-      </c>
-      <c r="T7" s="4" t="inlineStr">
-        <is>
-          <t>Back &amp; Biceps</t>
-        </is>
-      </c>
-      <c r="W7" s="3" t="inlineStr">
-        <is>
-          <t>Workout:</t>
-        </is>
-      </c>
-      <c r="X7" s="4" t="inlineStr">
-        <is>
-          <t>Legs &amp; Shoulders</t>
+          <t>asdasd</t>
         </is>
       </c>
     </row>
@@ -749,51 +650,6 @@
           <t>Reps</t>
         </is>
       </c>
-      <c r="O9" s="5" t="inlineStr">
-        <is>
-          <t>Exercises</t>
-        </is>
-      </c>
-      <c r="P9" s="5" t="inlineStr">
-        <is>
-          <t>Sets</t>
-        </is>
-      </c>
-      <c r="Q9" s="5" t="inlineStr">
-        <is>
-          <t>Reps</t>
-        </is>
-      </c>
-      <c r="S9" s="5" t="inlineStr">
-        <is>
-          <t>Exercises</t>
-        </is>
-      </c>
-      <c r="T9" s="5" t="inlineStr">
-        <is>
-          <t>Sets</t>
-        </is>
-      </c>
-      <c r="U9" s="5" t="inlineStr">
-        <is>
-          <t>Reps</t>
-        </is>
-      </c>
-      <c r="W9" s="5" t="inlineStr">
-        <is>
-          <t>Exercises</t>
-        </is>
-      </c>
-      <c r="X9" s="5" t="inlineStr">
-        <is>
-          <t>Sets</t>
-        </is>
-      </c>
-      <c r="Y9" s="5" t="inlineStr">
-        <is>
-          <t>Reps</t>
-        </is>
-      </c>
     </row>
     <row r="10">
       <c r="C10" s="6" t="inlineStr">
@@ -803,153 +659,121 @@
       </c>
       <c r="D10" s="6" t="inlineStr">
         <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E10" s="6" t="inlineStr">
+        <is>
+          <t>5-7</t>
+        </is>
+      </c>
+      <c r="G10" s="6" t="inlineStr">
+        <is>
+          <t>Squat</t>
+        </is>
+      </c>
+      <c r="H10" s="6" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="I10" s="6" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="K10" s="6" t="inlineStr">
+        <is>
+          <t>asdasd</t>
+        </is>
+      </c>
+      <c r="L10" s="6" t="inlineStr">
+        <is>
           <t>4</t>
         </is>
       </c>
-      <c r="E10" s="6" t="inlineStr">
-        <is>
-          <t>8-12</t>
-        </is>
-      </c>
-      <c r="G10" s="6" t="inlineStr">
+      <c r="M10" s="6" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="C11" s="6" t="inlineStr">
         <is>
           <t>Incline Bench Press</t>
         </is>
       </c>
-      <c r="H10" s="6" t="inlineStr">
+      <c r="D11" s="6" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="I10" s="6" t="inlineStr">
-        <is>
-          <t>4-6</t>
-        </is>
-      </c>
-      <c r="K10" s="6" t="inlineStr">
-        <is>
-          <t>Box style</t>
-        </is>
-      </c>
-      <c r="L10" s="6" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="M10" s="6" t="inlineStr">
-        <is>
-          <t>8-12</t>
-        </is>
-      </c>
-      <c r="O10" s="6" t="inlineStr">
-        <is>
-          <t>Jog2</t>
-        </is>
-      </c>
-      <c r="P10" s="6" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="Q10" s="6" t="inlineStr">
-        <is>
-          <t>4-6</t>
-        </is>
-      </c>
-      <c r="S10" s="6" t="inlineStr">
-        <is>
-          <t>Jog3</t>
-        </is>
-      </c>
-      <c r="T10" s="6" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="U10" s="6" t="inlineStr">
-        <is>
-          <t>4-6</t>
-        </is>
-      </c>
-      <c r="W10" s="6" t="inlineStr">
-        <is>
-          <t>Jog4</t>
-        </is>
-      </c>
-      <c r="X10" s="6" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="Y10" s="6" t="inlineStr">
-        <is>
-          <t>4-6</t>
+      <c r="E11" s="6" t="inlineStr">
+        <is>
+          <t>5-7</t>
         </is>
       </c>
     </row>
-    <row r="11"/>
     <row r="12"/>
     <row r="13"/>
     <row r="14"/>
     <row r="15"/>
     <row r="16"/>
     <row r="17">
-      <c r="W17" s="3" t="inlineStr">
+      <c r="C17" s="3" t="inlineStr">
         <is>
           <t>Workout:</t>
         </is>
       </c>
-      <c r="X17" s="4" t="inlineStr">
-        <is>
-          <t>Abs</t>
+      <c r="D17" s="4" t="inlineStr">
+        <is>
+          <t>Triceps</t>
         </is>
       </c>
     </row>
     <row r="18"/>
     <row r="19">
-      <c r="W19" s="5" t="inlineStr">
+      <c r="C19" s="5" t="inlineStr">
         <is>
           <t>Exercises</t>
         </is>
       </c>
-      <c r="X19" s="5" t="inlineStr">
+      <c r="D19" s="5" t="inlineStr">
         <is>
           <t>Sets</t>
         </is>
       </c>
-      <c r="Y19" s="5" t="inlineStr">
+      <c r="E19" s="5" t="inlineStr">
         <is>
           <t>Reps</t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="W20" s="6" t="inlineStr">
-        <is>
-          <t>Jog5</t>
-        </is>
-      </c>
-      <c r="X20" s="6" t="inlineStr">
+      <c r="C20" s="6" t="inlineStr">
+        <is>
+          <t>Overhead Extension</t>
+        </is>
+      </c>
+      <c r="D20" s="6" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="Y20" s="6" t="inlineStr">
-        <is>
-          <t>4-6</t>
+      <c r="E20" s="6" t="inlineStr">
+        <is>
+          <t>8-12</t>
         </is>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <tableParts count="7">
+  <tableParts count="4">
     <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
     <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
     <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
     <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
-    <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
-    <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
-    <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>